<commit_message>
Added code in Reusable methods
</commit_message>
<xml_diff>
--- a/DataSheet/Appium.xlsx
+++ b/DataSheet/Appium.xlsx
@@ -145,9 +145,6 @@
     <t>com.example.android.apis.ApiDemos</t>
   </si>
   <si>
-    <t>4.4.2</t>
-  </si>
-  <si>
     <t>com.android.browser</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>com.android.vending.AssetBrowserActivity</t>
+  </si>
+  <si>
+    <t>8.1.0</t>
   </si>
 </sst>
 </file>
@@ -524,14 +524,14 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
@@ -558,19 +558,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="K37" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L37" t="s">
         <v>34</v>
@@ -637,18 +637,18 @@
         <v>36</v>
       </c>
       <c r="L39" t="s">
+        <v>39</v>
+      </c>
+      <c r="M39" t="s">
         <v>40</v>
-      </c>
-      <c r="M39" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="40" spans="9:13" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
+        <v>41</v>
+      </c>
+      <c r="M40" t="s">
         <v>42</v>
-      </c>
-      <c r="M40" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new apk file
</commit_message>
<xml_diff>
--- a/DataSheet/Appium.xlsx
+++ b/DataSheet/Appium.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>LeaveType</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>8.1.0</t>
+  </si>
+  <si>
+    <t>io.selendroid.testapp.HomeScreenActivity</t>
+  </si>
+  <si>
+    <t>io.selendroid.testapp</t>
   </si>
 </sst>
 </file>
@@ -521,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,10 +571,10 @@
         <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="9:13" x14ac:dyDescent="0.25">
@@ -647,6 +653,14 @@
       </c>
       <c r="M40" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>45</v>
+      </c>
+      <c r="M41" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>